<commit_message>
feat: LWT ebay 删减列
</commit_message>
<xml_diff>
--- a/template/ebay.xlsx
+++ b/template/ebay.xlsx
@@ -4,18 +4,31 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15640"/>
+    <workbookView windowWidth="30880" windowHeight="14820"/>
   </bookViews>
   <sheets>
-    <sheet name="LWT for Amzon" sheetId="1" r:id="rId1"/>
+    <sheet name="LWT for Ebay" sheetId="1" r:id="rId1"/>
     <sheet name="公式模版" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="105">
   <si>
     <t>European eBay Declared Value-Analysis Report(v2.0)</t>
   </si>
@@ -69,9 +82,6 @@
     <t>eBay cost(In Euro)</t>
   </si>
   <si>
-    <t>Profit</t>
-  </si>
-  <si>
     <t>LOCAL Cost(Euro/ KG)</t>
   </si>
   <si>
@@ -114,12 +124,6 @@
     <t>Commission Fees</t>
   </si>
   <si>
-    <t>Closing Fee</t>
-  </si>
-  <si>
-    <t>High volume lising Fee</t>
-  </si>
-  <si>
     <t>PayPal Processing rate</t>
   </si>
   <si>
@@ -145,12 +149,6 @@
   </si>
   <si>
     <t>Storage Fee</t>
-  </si>
-  <si>
-    <t>Advertising Fee</t>
-  </si>
-  <si>
-    <t>Profit Rate</t>
   </si>
   <si>
     <t>Ground Service Rate</t>
@@ -405,6 +403,9 @@
     <t>Amazon cost(In Euro)</t>
   </si>
   <si>
+    <t>Profit</t>
+  </si>
+  <si>
     <t>NL LOCAL Cost(Euro/ KG)</t>
   </si>
   <si>
@@ -423,6 +424,12 @@
     <t>Referral Fees</t>
   </si>
   <si>
+    <t>Closing Fee</t>
+  </si>
+  <si>
+    <t>High volume lising Fee</t>
+  </si>
+  <si>
     <t>Processing rate</t>
   </si>
   <si>
@@ -436,6 +443,12 @@
   </si>
   <si>
     <t>Fulfillment fee</t>
+  </si>
+  <si>
+    <t>Advertising Fee</t>
+  </si>
+  <si>
+    <t>Profit Rate</t>
   </si>
   <si>
     <t>Ground Sercice Rate</t>
@@ -474,19 +487,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="11">
-    <numFmt numFmtId="176" formatCode="0.000000"/>
-    <numFmt numFmtId="177" formatCode="#,##0.00&quot; &quot;"/>
-    <numFmt numFmtId="178" formatCode="0.0000"/>
-    <numFmt numFmtId="179" formatCode="#,##0&quot; &quot;"/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="0.00000000&quot; &quot;"/>
-    <numFmt numFmtId="181" formatCode="0.00&quot; &quot;"/>
-    <numFmt numFmtId="182" formatCode="0.000"/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="#,##0&quot; &quot;"/>
+    <numFmt numFmtId="177" formatCode="0.00&quot; &quot;"/>
+    <numFmt numFmtId="178" formatCode="0.00000000&quot; &quot;"/>
+    <numFmt numFmtId="179" formatCode="0.0000"/>
+    <numFmt numFmtId="180" formatCode="#,##0.00&quot; &quot;"/>
+    <numFmt numFmtId="181" formatCode="0.000000"/>
+    <numFmt numFmtId="182" formatCode="0.000"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -534,37 +547,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Helvetica Neue"/>
@@ -572,11 +554,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -604,16 +601,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -628,7 +649,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -642,44 +692,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -719,13 +732,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -737,43 +750,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -785,7 +762,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -803,7 +780,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -815,13 +870,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -833,73 +900,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1071,41 +1084,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1130,17 +1108,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1160,6 +1132,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1168,151 +1170,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1339,7 +1352,7 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1348,18 +1361,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="181" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="180" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1372,13 +1385,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1450,69 +1463,69 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="181" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="181" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="181" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
-    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
-    <cellStyle name="输入" xfId="4" builtinId="20"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
-    <cellStyle name="货币" xfId="7" builtinId="4"/>
-    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
-    <cellStyle name="百分比" xfId="9" builtinId="5"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
-    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
-    <cellStyle name="计算" xfId="15" builtinId="22"/>
-    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
-    <cellStyle name="适中" xfId="17" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
-    <cellStyle name="好" xfId="19" builtinId="26"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
     <cellStyle name="汇总" xfId="21" builtinId="25"/>
-    <cellStyle name="差" xfId="22" builtinId="27"/>
-    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
-    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
-    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
-    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
-    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
-    <cellStyle name="标题" xfId="33" builtinId="15"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
-    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
     <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
-    <cellStyle name="注释" xfId="37" builtinId="10"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
-    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8"/>
-    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
-    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
-    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <tableStyles count="0"/>
   <colors>
@@ -1779,13 +1792,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>547839</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>223287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>69378</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>269783</xdr:rowOff>
@@ -1797,7 +1810,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16835755" y="661035"/>
+          <a:off x="15921990" y="661035"/>
           <a:ext cx="197485" cy="382905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1871,13 +1884,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>624111</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>227732</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>18506</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>274228</xdr:rowOff>
@@ -1889,7 +1902,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="18263235" y="665480"/>
+          <a:off x="17349470" y="665480"/>
           <a:ext cx="177165" cy="382905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1963,13 +1976,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>982027</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>220112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>206686</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>266608</xdr:rowOff>
@@ -1981,7 +1994,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="21148675" y="657860"/>
+          <a:off x="20234910" y="657860"/>
           <a:ext cx="206375" cy="382905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2055,13 +2068,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>31</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>472211</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>204036</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
+      <xdr:col>30</xdr:col>
       <xdr:colOff>204870</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>250532</xdr:rowOff>
@@ -2073,7 +2086,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="22285325" y="641985"/>
+          <a:off x="21371560" y="641985"/>
           <a:ext cx="230505" cy="382905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3187,10 +3200,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:BA17"/>
+  <dimension ref="A1:AV17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AP30" sqref="AP30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83035714285714" defaultRowHeight="14" customHeight="1"/>
@@ -3210,35 +3223,32 @@
     <col min="20" max="20" width="10.5" style="1" customWidth="1"/>
     <col min="21" max="21" width="12.5" style="1" customWidth="1"/>
     <col min="22" max="22" width="12.8482142857143" style="1" customWidth="1"/>
-    <col min="23" max="23" width="6.34821428571429" style="1" customWidth="1"/>
-    <col min="24" max="24" width="6.5" style="1" customWidth="1"/>
-    <col min="25" max="26" width="9.5" style="1" customWidth="1"/>
-    <col min="27" max="28" width="11" style="1" customWidth="1"/>
-    <col min="29" max="30" width="13.6696428571429" style="1" customWidth="1"/>
-    <col min="31" max="31" width="9.34821428571429" style="1" customWidth="1"/>
-    <col min="32" max="33" width="7" style="1" customWidth="1"/>
-    <col min="34" max="34" width="9.34821428571429" style="1" customWidth="1"/>
-    <col min="35" max="35" width="5.5" style="1" customWidth="1"/>
-    <col min="36" max="36" width="6" style="1" customWidth="1"/>
-    <col min="37" max="37" width="10" style="1" customWidth="1"/>
-    <col min="38" max="38" width="8.84821428571429" style="1" customWidth="1"/>
+    <col min="23" max="24" width="9.5" style="1" customWidth="1"/>
+    <col min="25" max="26" width="11" style="1" customWidth="1"/>
+    <col min="27" max="28" width="13.6696428571429" style="1" customWidth="1"/>
+    <col min="29" max="29" width="9.34821428571429" style="1" customWidth="1"/>
+    <col min="30" max="31" width="7" style="1" customWidth="1"/>
+    <col min="32" max="32" width="10" style="1" customWidth="1"/>
+    <col min="33" max="33" width="8.84821428571429" style="1" customWidth="1"/>
+    <col min="34" max="34" width="10.6696428571429" style="1" customWidth="1"/>
+    <col min="35" max="35" width="11.3482142857143" style="1" customWidth="1"/>
+    <col min="36" max="37" width="10.6696428571429" style="1" customWidth="1"/>
+    <col min="38" max="38" width="9" style="1" customWidth="1"/>
     <col min="39" max="39" width="10.6696428571429" style="1" customWidth="1"/>
-    <col min="40" max="40" width="11.3482142857143" style="1" customWidth="1"/>
-    <col min="41" max="42" width="10.6696428571429" style="1" customWidth="1"/>
-    <col min="43" max="43" width="9" style="1" customWidth="1"/>
-    <col min="44" max="44" width="10.6696428571429" style="1" customWidth="1"/>
-    <col min="45" max="46" width="13" style="1" customWidth="1"/>
-    <col min="47" max="47" width="9" style="1" customWidth="1"/>
-    <col min="48" max="48" width="14.8482142857143" style="1" customWidth="1"/>
-    <col min="49" max="49" width="19" style="1" customWidth="1"/>
-    <col min="50" max="50" width="8" style="1" customWidth="1"/>
-    <col min="51" max="51" width="8.5" style="1" customWidth="1"/>
-    <col min="52" max="52" width="9.84821428571429" style="1" customWidth="1"/>
-    <col min="53" max="53" width="13.8482142857143" style="1" customWidth="1"/>
-    <col min="54" max="16384" width="8.84821428571429" style="1" customWidth="1"/>
+    <col min="40" max="41" width="13" style="1" customWidth="1"/>
+    <col min="42" max="42" width="9" style="1" customWidth="1"/>
+    <col min="43" max="43" width="14.8482142857143" style="1" customWidth="1"/>
+    <col min="44" max="44" width="19" style="1" customWidth="1"/>
+    <col min="45" max="45" width="8" style="1" customWidth="1"/>
+    <col min="46" max="46" width="8.5" style="1" customWidth="1"/>
+    <col min="47" max="47" width="9.84821428571429" style="1" customWidth="1"/>
+    <col min="48" max="48" width="13.8482142857143" style="1" customWidth="1"/>
+    <col min="49" max="16379" width="8.84821428571429" style="1" customWidth="1"/>
+    <col min="16380" max="16380" width="8.84821428571429" style="1"/>
+    <col min="16381" max="16384" width="8.83035714285714" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="34.5" customHeight="1" spans="1:53">
+    <row r="1" ht="34.5" customHeight="1" spans="1:48">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3287,15 +3297,10 @@
       <c r="AR1" s="5"/>
       <c r="AS1" s="5"/>
       <c r="AT1" s="5"/>
-      <c r="AU1" s="5"/>
-      <c r="AV1" s="5"/>
-      <c r="AW1" s="5"/>
-      <c r="AX1" s="5"/>
-      <c r="AY1" s="5"/>
-      <c r="AZ1" s="24"/>
-      <c r="BA1" s="65"/>
+      <c r="AU1" s="24"/>
+      <c r="AV1" s="62"/>
     </row>
-    <row r="2" ht="26.5" customHeight="1" spans="1:53">
+    <row r="2" ht="26.5" customHeight="1" spans="1:48">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -3359,42 +3364,35 @@
       <c r="AC2" s="7"/>
       <c r="AD2" s="7"/>
       <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
+      <c r="AF2" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="AG2" s="7"/>
       <c r="AH2" s="7"/>
-      <c r="AI2" s="6" t="s">
-        <v>17</v>
-      </c>
+      <c r="AI2" s="7"/>
       <c r="AJ2" s="7"/>
-      <c r="AK2" s="6" t="s">
-        <v>18</v>
-      </c>
+      <c r="AK2" s="7"/>
       <c r="AL2" s="7"/>
       <c r="AM2" s="7"/>
       <c r="AN2" s="7"/>
       <c r="AO2" s="7"/>
       <c r="AP2" s="7"/>
-      <c r="AQ2" s="7"/>
-      <c r="AR2" s="7"/>
-      <c r="AS2" s="7"/>
+      <c r="AQ2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AR2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS2" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="AT2" s="7"/>
       <c r="AU2" s="7"/>
-      <c r="AV2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="AW2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="AX2" s="6" t="s">
+      <c r="AV2" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="AY2" s="7"/>
-      <c r="AZ2" s="7"/>
-      <c r="BA2" s="30" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="3" ht="60" customHeight="1" spans="1:53">
+    <row r="3" ht="60" customHeight="1" spans="1:48">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -3409,73 +3407,73 @@
       <c r="L3" s="17"/>
       <c r="M3" s="7"/>
       <c r="N3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="P3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="21" t="s">
+      <c r="V3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="Y3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="Z3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="AA3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AB3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AB3" s="6" t="s">
+      <c r="AC3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AD3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AD3" s="6" t="s">
+      <c r="AE3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AE3" s="6" t="s">
+      <c r="AF3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AF3" s="6" t="s">
+      <c r="AG3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AG3" s="6" t="s">
+      <c r="AH3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AH3" s="6" t="s">
+      <c r="AI3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AI3" s="6" t="s">
+      <c r="AJ3" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="AJ3" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="AK3" s="6" t="s">
         <v>45</v>
@@ -3495,35 +3493,20 @@
       <c r="AP3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="AQ3" s="6" t="s">
+      <c r="AQ3" s="7"/>
+      <c r="AR3" s="7"/>
+      <c r="AS3" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="AR3" s="6" t="s">
+      <c r="AT3" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="AS3" s="6" t="s">
+      <c r="AU3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="AT3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="AU3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="AV3" s="7"/>
-      <c r="AW3" s="7"/>
-      <c r="AX3" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AY3" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="AZ3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="BA3" s="31"/>
+      <c r="AV3" s="31"/>
     </row>
-    <row r="4" ht="14.25" customHeight="1" spans="1:53">
+    <row r="4" ht="14.25" customHeight="1" spans="1:48">
       <c r="A4" s="11"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -3546,39 +3529,34 @@
       <c r="T4" s="57"/>
       <c r="U4" s="12"/>
       <c r="V4" s="46"/>
-      <c r="W4" s="46"/>
+      <c r="W4" s="57"/>
       <c r="X4" s="46"/>
       <c r="Y4" s="57"/>
       <c r="Z4" s="46"/>
       <c r="AA4" s="57"/>
       <c r="AB4" s="46"/>
-      <c r="AC4" s="57"/>
-      <c r="AD4" s="46"/>
+      <c r="AC4" s="46"/>
+      <c r="AD4" s="57"/>
       <c r="AE4" s="46"/>
       <c r="AF4" s="57"/>
-      <c r="AG4" s="46"/>
-      <c r="AH4" s="46"/>
-      <c r="AI4" s="57"/>
+      <c r="AG4" s="57"/>
+      <c r="AH4" s="57"/>
+      <c r="AI4" s="46"/>
       <c r="AJ4" s="57"/>
-      <c r="AK4" s="57"/>
+      <c r="AK4" s="46"/>
       <c r="AL4" s="57"/>
-      <c r="AM4" s="57"/>
-      <c r="AN4" s="46"/>
+      <c r="AM4" s="46"/>
+      <c r="AN4" s="57"/>
       <c r="AO4" s="57"/>
-      <c r="AP4" s="46"/>
-      <c r="AQ4" s="57"/>
-      <c r="AR4" s="46"/>
+      <c r="AP4" s="57"/>
+      <c r="AQ4" s="12"/>
+      <c r="AR4" s="12"/>
       <c r="AS4" s="57"/>
-      <c r="AT4" s="57"/>
-      <c r="AU4" s="57"/>
-      <c r="AV4" s="12"/>
-      <c r="AW4" s="12"/>
-      <c r="AX4" s="57"/>
-      <c r="AY4" s="12"/>
-      <c r="AZ4" s="62"/>
-      <c r="BA4" s="66"/>
+      <c r="AT4" s="12"/>
+      <c r="AU4" s="63"/>
+      <c r="AV4" s="64"/>
     </row>
-    <row r="5" ht="14.25" customHeight="1" spans="1:53">
+    <row r="5" ht="14.25" customHeight="1" spans="1:48">
       <c r="A5" s="13"/>
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
@@ -3601,41 +3579,36 @@
       <c r="T5" s="58"/>
       <c r="U5" s="14"/>
       <c r="V5" s="48"/>
-      <c r="W5" s="48"/>
+      <c r="W5" s="58"/>
       <c r="X5" s="48"/>
       <c r="Y5" s="58"/>
       <c r="Z5" s="48"/>
       <c r="AA5" s="58"/>
       <c r="AB5" s="48"/>
-      <c r="AC5" s="58"/>
-      <c r="AD5" s="48"/>
+      <c r="AC5" s="48"/>
+      <c r="AD5" s="58"/>
       <c r="AE5" s="48"/>
       <c r="AF5" s="58"/>
-      <c r="AG5" s="48"/>
-      <c r="AH5" s="48"/>
-      <c r="AI5" s="58"/>
+      <c r="AG5" s="58"/>
+      <c r="AH5" s="58"/>
+      <c r="AI5" s="48"/>
       <c r="AJ5" s="58"/>
-      <c r="AK5" s="58"/>
+      <c r="AK5" s="48"/>
       <c r="AL5" s="58"/>
-      <c r="AM5" s="58"/>
-      <c r="AN5" s="48"/>
+      <c r="AM5" s="48"/>
+      <c r="AN5" s="58"/>
       <c r="AO5" s="58"/>
-      <c r="AP5" s="48"/>
-      <c r="AQ5" s="58"/>
-      <c r="AR5" s="48"/>
+      <c r="AP5" s="58"/>
+      <c r="AQ5" s="14"/>
+      <c r="AR5" s="14"/>
       <c r="AS5" s="58"/>
-      <c r="AT5" s="58"/>
-      <c r="AU5" s="58"/>
-      <c r="AV5" s="14"/>
-      <c r="AW5" s="14"/>
-      <c r="AX5" s="58"/>
-      <c r="AY5" s="14"/>
-      <c r="AZ5" s="63"/>
-      <c r="BA5" s="67"/>
+      <c r="AT5" s="14"/>
+      <c r="AU5" s="65"/>
+      <c r="AV5" s="66"/>
     </row>
-    <row r="6" ht="20.25" customHeight="1" spans="1:53">
+    <row r="6" ht="20.25" customHeight="1" spans="1:48">
       <c r="A6" s="36" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B6" s="37"/>
       <c r="C6" s="37"/>
@@ -3658,48 +3631,43 @@
       <c r="T6" s="58"/>
       <c r="U6" s="14"/>
       <c r="V6" s="48"/>
-      <c r="W6" s="48"/>
+      <c r="W6" s="58"/>
       <c r="X6" s="48"/>
       <c r="Y6" s="58"/>
       <c r="Z6" s="48"/>
       <c r="AA6" s="58"/>
       <c r="AB6" s="48"/>
-      <c r="AC6" s="58"/>
-      <c r="AD6" s="48"/>
+      <c r="AC6" s="48"/>
+      <c r="AD6" s="58"/>
       <c r="AE6" s="48"/>
       <c r="AF6" s="58"/>
-      <c r="AG6" s="48"/>
-      <c r="AH6" s="48"/>
-      <c r="AI6" s="58"/>
+      <c r="AG6" s="58"/>
+      <c r="AH6" s="58"/>
+      <c r="AI6" s="48"/>
       <c r="AJ6" s="58"/>
-      <c r="AK6" s="58"/>
+      <c r="AK6" s="48"/>
       <c r="AL6" s="58"/>
-      <c r="AM6" s="58"/>
-      <c r="AN6" s="48"/>
+      <c r="AM6" s="48"/>
+      <c r="AN6" s="58"/>
       <c r="AO6" s="58"/>
-      <c r="AP6" s="48"/>
-      <c r="AQ6" s="58"/>
-      <c r="AR6" s="48"/>
+      <c r="AP6" s="58"/>
+      <c r="AQ6" s="14"/>
+      <c r="AR6" s="14"/>
       <c r="AS6" s="58"/>
-      <c r="AT6" s="58"/>
-      <c r="AU6" s="58"/>
-      <c r="AV6" s="14"/>
-      <c r="AW6" s="14"/>
-      <c r="AX6" s="58"/>
-      <c r="AY6" s="14"/>
-      <c r="AZ6" s="63"/>
-      <c r="BA6" s="67"/>
+      <c r="AT6" s="14"/>
+      <c r="AU6" s="65"/>
+      <c r="AV6" s="66"/>
     </row>
-    <row r="7" ht="16.5" customHeight="1" spans="1:53">
+    <row r="7" ht="16.5" customHeight="1" spans="1:48">
       <c r="A7" s="39" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B7" s="37"/>
       <c r="C7" s="40" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="37"/>
@@ -3744,23 +3712,18 @@
       <c r="AS7" s="14"/>
       <c r="AT7" s="14"/>
       <c r="AU7" s="14"/>
-      <c r="AV7" s="14"/>
-      <c r="AW7" s="14"/>
-      <c r="AX7" s="14"/>
-      <c r="AY7" s="14"/>
-      <c r="AZ7" s="14"/>
-      <c r="BA7" s="34"/>
+      <c r="AV7" s="34"/>
     </row>
-    <row r="8" ht="16.5" customHeight="1" spans="1:53">
+    <row r="8" ht="16.5" customHeight="1" spans="1:48">
       <c r="A8" s="39" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B8" s="37"/>
       <c r="C8" s="40" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="37"/>
@@ -3805,23 +3768,18 @@
       <c r="AS8" s="14"/>
       <c r="AT8" s="14"/>
       <c r="AU8" s="14"/>
-      <c r="AV8" s="14"/>
-      <c r="AW8" s="14"/>
-      <c r="AX8" s="14"/>
-      <c r="AY8" s="14"/>
-      <c r="AZ8" s="14"/>
-      <c r="BA8" s="34"/>
+      <c r="AV8" s="34"/>
     </row>
-    <row r="9" ht="16.5" customHeight="1" spans="1:53">
+    <row r="9" ht="16.5" customHeight="1" spans="1:48">
       <c r="A9" s="39" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B9" s="37"/>
       <c r="C9" s="40" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
@@ -3866,21 +3824,16 @@
       <c r="AS9" s="14"/>
       <c r="AT9" s="14"/>
       <c r="AU9" s="14"/>
-      <c r="AV9" s="14"/>
-      <c r="AW9" s="14"/>
-      <c r="AX9" s="14"/>
-      <c r="AY9" s="14"/>
-      <c r="AZ9" s="14"/>
-      <c r="BA9" s="34"/>
+      <c r="AV9" s="34"/>
     </row>
-    <row r="10" ht="15" customHeight="1" spans="1:53">
+    <row r="10" ht="15" customHeight="1" spans="1:48">
       <c r="A10" s="39" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B10" s="37"/>
       <c r="C10" s="38"/>
       <c r="D10" s="41" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="37"/>
@@ -3925,16 +3878,11 @@
       <c r="AS10" s="14"/>
       <c r="AT10" s="14"/>
       <c r="AU10" s="14"/>
-      <c r="AV10" s="14"/>
-      <c r="AW10" s="14"/>
-      <c r="AX10" s="14"/>
-      <c r="AY10" s="14"/>
-      <c r="AZ10" s="14"/>
-      <c r="BA10" s="34"/>
+      <c r="AV10" s="34"/>
     </row>
-    <row r="11" ht="15" customHeight="1" spans="1:53">
+    <row r="11" ht="15" customHeight="1" spans="1:48">
       <c r="A11" s="39" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B11" s="37"/>
       <c r="C11" s="38"/>
@@ -3982,16 +3930,11 @@
       <c r="AS11" s="14"/>
       <c r="AT11" s="14"/>
       <c r="AU11" s="14"/>
-      <c r="AV11" s="14"/>
-      <c r="AW11" s="14"/>
-      <c r="AX11" s="14"/>
-      <c r="AY11" s="14"/>
-      <c r="AZ11" s="14"/>
-      <c r="BA11" s="34"/>
+      <c r="AV11" s="34"/>
     </row>
-    <row r="12" ht="15" customHeight="1" spans="1:53">
+    <row r="12" ht="15" customHeight="1" spans="1:48">
       <c r="A12" s="39" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B12" s="37"/>
       <c r="C12" s="38"/>
@@ -4039,23 +3982,18 @@
       <c r="AS12" s="14"/>
       <c r="AT12" s="14"/>
       <c r="AU12" s="14"/>
-      <c r="AV12" s="14"/>
-      <c r="AW12" s="14"/>
-      <c r="AX12" s="14"/>
-      <c r="AY12" s="14"/>
-      <c r="AZ12" s="14"/>
-      <c r="BA12" s="34"/>
+      <c r="AV12" s="34"/>
     </row>
-    <row r="13" ht="16.5" customHeight="1" spans="1:53">
+    <row r="13" ht="16.5" customHeight="1" spans="1:48">
       <c r="A13" s="39" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B13" s="37"/>
       <c r="C13" s="40" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D13" s="41" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E13" s="37"/>
       <c r="F13" s="37"/>
@@ -4100,19 +4038,14 @@
       <c r="AS13" s="14"/>
       <c r="AT13" s="14"/>
       <c r="AU13" s="14"/>
-      <c r="AV13" s="14"/>
-      <c r="AW13" s="14"/>
-      <c r="AX13" s="14"/>
-      <c r="AY13" s="14"/>
-      <c r="AZ13" s="14"/>
-      <c r="BA13" s="34"/>
+      <c r="AV13" s="34"/>
     </row>
-    <row r="14" ht="15" customHeight="1" spans="1:53">
+    <row r="14" ht="15" customHeight="1" spans="1:48">
       <c r="A14" s="13"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
       <c r="D14" s="41" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -4157,20 +4090,15 @@
       <c r="AS14" s="14"/>
       <c r="AT14" s="14"/>
       <c r="AU14" s="14"/>
-      <c r="AV14" s="14"/>
-      <c r="AW14" s="14"/>
-      <c r="AX14" s="14"/>
-      <c r="AY14" s="14"/>
-      <c r="AZ14" s="14"/>
-      <c r="BA14" s="34"/>
+      <c r="AV14" s="34"/>
     </row>
-    <row r="15" ht="16.5" customHeight="1" spans="1:53">
+    <row r="15" ht="16.5" customHeight="1" spans="1:48">
       <c r="A15" s="39" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B15" s="37"/>
       <c r="C15" s="40" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D15" s="42"/>
       <c r="E15" s="37"/>
@@ -4216,14 +4144,9 @@
       <c r="AS15" s="14"/>
       <c r="AT15" s="14"/>
       <c r="AU15" s="14"/>
-      <c r="AV15" s="14"/>
-      <c r="AW15" s="14"/>
-      <c r="AX15" s="14"/>
-      <c r="AY15" s="14"/>
-      <c r="AZ15" s="14"/>
-      <c r="BA15" s="34"/>
+      <c r="AV15" s="34"/>
     </row>
-    <row r="16" ht="15" customHeight="1" spans="1:53">
+    <row r="16" ht="15" customHeight="1" spans="1:48">
       <c r="A16" s="43"/>
       <c r="B16" s="38"/>
       <c r="C16" s="40"/>
@@ -4246,39 +4169,34 @@
       <c r="T16" s="58"/>
       <c r="U16" s="14"/>
       <c r="V16" s="48"/>
-      <c r="W16" s="48"/>
+      <c r="W16" s="58"/>
       <c r="X16" s="48"/>
       <c r="Y16" s="58"/>
       <c r="Z16" s="48"/>
       <c r="AA16" s="58"/>
       <c r="AB16" s="48"/>
-      <c r="AC16" s="58"/>
-      <c r="AD16" s="48"/>
+      <c r="AC16" s="48"/>
+      <c r="AD16" s="58"/>
       <c r="AE16" s="48"/>
       <c r="AF16" s="58"/>
-      <c r="AG16" s="48"/>
-      <c r="AH16" s="48"/>
-      <c r="AI16" s="58"/>
+      <c r="AG16" s="58"/>
+      <c r="AH16" s="58"/>
+      <c r="AI16" s="48"/>
       <c r="AJ16" s="58"/>
-      <c r="AK16" s="58"/>
+      <c r="AK16" s="48"/>
       <c r="AL16" s="58"/>
-      <c r="AM16" s="58"/>
-      <c r="AN16" s="48"/>
+      <c r="AM16" s="48"/>
+      <c r="AN16" s="58"/>
       <c r="AO16" s="58"/>
-      <c r="AP16" s="48"/>
-      <c r="AQ16" s="58"/>
-      <c r="AR16" s="48"/>
+      <c r="AP16" s="58"/>
+      <c r="AQ16" s="14"/>
+      <c r="AR16" s="14"/>
       <c r="AS16" s="58"/>
-      <c r="AT16" s="58"/>
-      <c r="AU16" s="58"/>
-      <c r="AV16" s="14"/>
-      <c r="AW16" s="14"/>
-      <c r="AX16" s="58"/>
-      <c r="AY16" s="14"/>
-      <c r="AZ16" s="63"/>
-      <c r="BA16" s="67"/>
+      <c r="AT16" s="14"/>
+      <c r="AU16" s="65"/>
+      <c r="AV16" s="66"/>
     </row>
-    <row r="17" ht="25.5" customHeight="1" spans="1:53">
+    <row r="17" ht="25.5" customHeight="1" spans="1:48">
       <c r="A17" s="44"/>
       <c r="B17" s="45"/>
       <c r="C17" s="45"/>
@@ -4287,14 +4205,14 @@
       <c r="F17" s="55"/>
       <c r="G17" s="55"/>
       <c r="H17" s="56" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="I17" s="16"/>
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
       <c r="L17" s="16"/>
       <c r="M17" s="59" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="N17" s="60"/>
       <c r="O17" s="61"/>
@@ -4305,47 +4223,41 @@
       <c r="T17" s="60"/>
       <c r="U17" s="16"/>
       <c r="V17" s="61"/>
-      <c r="W17" s="61"/>
+      <c r="W17" s="60"/>
       <c r="X17" s="61"/>
       <c r="Y17" s="60"/>
       <c r="Z17" s="61"/>
       <c r="AA17" s="60"/>
       <c r="AB17" s="61"/>
-      <c r="AC17" s="60"/>
-      <c r="AD17" s="61"/>
+      <c r="AC17" s="61"/>
+      <c r="AD17" s="60"/>
       <c r="AE17" s="61"/>
       <c r="AF17" s="60"/>
-      <c r="AG17" s="61"/>
-      <c r="AH17" s="61"/>
-      <c r="AI17" s="60"/>
+      <c r="AG17" s="60"/>
+      <c r="AH17" s="60"/>
+      <c r="AI17" s="61"/>
       <c r="AJ17" s="60"/>
-      <c r="AK17" s="60"/>
+      <c r="AK17" s="61"/>
       <c r="AL17" s="60"/>
-      <c r="AM17" s="60"/>
-      <c r="AN17" s="61"/>
+      <c r="AM17" s="61"/>
+      <c r="AN17" s="60"/>
       <c r="AO17" s="60"/>
-      <c r="AP17" s="61"/>
-      <c r="AQ17" s="60"/>
-      <c r="AR17" s="61"/>
+      <c r="AP17" s="60"/>
+      <c r="AQ17" s="16"/>
+      <c r="AR17" s="16"/>
       <c r="AS17" s="60"/>
-      <c r="AT17" s="60"/>
-      <c r="AU17" s="60"/>
-      <c r="AV17" s="16"/>
-      <c r="AW17" s="16"/>
-      <c r="AX17" s="60"/>
-      <c r="AY17" s="16"/>
-      <c r="AZ17" s="64"/>
-      <c r="BA17" s="68"/>
+      <c r="AT17" s="16"/>
+      <c r="AU17" s="67"/>
+      <c r="AV17" s="68"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="A1:AZ1"/>
+  <mergeCells count="22">
+    <mergeCell ref="A1:AU1"/>
     <mergeCell ref="N2:Q2"/>
     <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AK2:AU2"/>
-    <mergeCell ref="AX2:AZ2"/>
+    <mergeCell ref="T2:AE2"/>
+    <mergeCell ref="AF2:AP2"/>
+    <mergeCell ref="AS2:AU2"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -4359,9 +4271,9 @@
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="M2:M3"/>
+    <mergeCell ref="AQ2:AQ3"/>
+    <mergeCell ref="AR2:AR3"/>
     <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="AW2:AW3"/>
-    <mergeCell ref="BA2:BA3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId2" display="https://www.belastingdienst.nl/rekenhulpen/wisselkoersen/"/>
@@ -4493,7 +4405,7 @@
     </row>
     <row r="2" ht="34.5" customHeight="1" spans="1:53">
       <c r="A2" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -4553,7 +4465,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>3</v>
@@ -4580,7 +4492,7 @@
         <v>10</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>12</v>
@@ -4589,7 +4501,7 @@
         <v>13</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
@@ -4599,7 +4511,7 @@
       </c>
       <c r="S3" s="7"/>
       <c r="T3" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="U3" s="7"/>
       <c r="V3" s="7"/>
@@ -4616,11 +4528,11 @@
       <c r="AG3" s="7"/>
       <c r="AH3" s="7"/>
       <c r="AI3" s="6" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="AJ3" s="7"/>
       <c r="AK3" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="AL3" s="7"/>
       <c r="AM3" s="7"/>
@@ -4633,18 +4545,18 @@
       <c r="AT3" s="7"/>
       <c r="AU3" s="7"/>
       <c r="AV3" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AW3" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="AX3" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="AY3" s="7"/>
       <c r="AZ3" s="7"/>
       <c r="BA3" s="30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" ht="60" customHeight="1" spans="1:53">
@@ -4662,73 +4574,73 @@
       <c r="L4" s="17"/>
       <c r="M4" s="7"/>
       <c r="N4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="Q4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="R4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="S4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S4" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="T4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="U4" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="X4" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="U4" s="21" t="s">
+      <c r="Y4" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="V4" s="6" t="s">
+      <c r="Z4" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="W4" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="X4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y4" s="6" t="s">
+      <c r="AA4" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="Z4" s="6" t="s">
+      <c r="AB4" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="AA4" s="6" t="s">
+      <c r="AC4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE4" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="AB4" s="6" t="s">
+      <c r="AF4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH4" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="AC4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD4" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE4" s="6" t="s">
+      <c r="AI4" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="AF4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG4" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="AH4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI4" s="6" t="s">
-        <v>44</v>
-      </c>
       <c r="AJ4" s="6" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="AK4" s="6" t="s">
         <v>94</v>
@@ -4737,31 +4649,31 @@
         <v>95</v>
       </c>
       <c r="AM4" s="6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="AN4" s="6" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="AO4" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="AP4" s="6" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="AQ4" s="6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="AR4" s="6" t="s">
         <v>96</v>
       </c>
       <c r="AS4" s="6" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="AT4" s="6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="AU4" s="6" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="AV4" s="7"/>
       <c r="AW4" s="7"/>

</xml_diff>